<commit_message>
Complte Yearly report practice
</commit_message>
<xml_diff>
--- a/WorkItems.xlsx
+++ b/WorkItems.xlsx
@@ -5,10 +5,10 @@
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhashimk\Documents\UiPath\Calculate Client Security Hash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhashimk\Documents\UiPath\Generate Yearly Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4152A224-9FCD-4DB4-858B-C46AD1A6A480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194ACD6B-252F-475D-920A-016E70E9EFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <x:si>
     <x:t>Actions Url</x:t>
   </x:si>
@@ -41,160 +41,67 @@
     <x:t>Date</x:t>
   </x:si>
   <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094305</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094305</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Calculate Client Security Hash</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WI5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Completed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2018-03-21</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094312</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094312</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2023-02-23</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094317</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094317</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2022-11-23</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094318</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094318</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2018-03-19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094313</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094313</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2023-03-10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094308</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094308</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-06-16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094320</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094320</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2019-10-25</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094310</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094310</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2022-12-16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094316</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094316</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2018-02-27</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094311</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094311</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2023-04-19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094309</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094309</x:t>
+    <x:t>https://acme-test.uipath.com/work-items/95094332</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95094332</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Generate Yearly Report for Vendor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WI4</x:t>
   </x:si>
   <x:si>
     <x:t>Open</x:t>
   </x:si>
   <x:si>
-    <x:t>2021-06-05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094315</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094315</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2019-04-07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094319</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094319</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2022-08-12</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094306</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094306</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2019-01-28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094314</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094314</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-03-25</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/95094307</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95094307</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2021-08-30</x:t>
+    <x:t>2022-12-25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://acme-test.uipath.com/work-items/95094323</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95094323</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2022-09-24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://acme-test.uipath.com/work-items/95094331</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95094331</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2022-06-29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://acme-test.uipath.com/work-items/95094326</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95094326</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2020-12-09</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://acme-test.uipath.com/work-items/95094321</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95094321</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-11-10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://acme-test.uipath.com/work-items/95094324</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95094324</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-04-03</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -541,12 +448,15 @@
   <x:dimension ref="A1"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="L11" sqref="L11"/>
+      <x:selection activeCell="J12" sqref="J12"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="18.425781" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:12">
+    <x:row r="1" spans="1:10">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -566,7 +476,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:12">
+    <x:row r="2" spans="1:10">
       <x:c r="A2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -586,7 +496,7 @@
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:12">
+    <x:row r="3" spans="1:10">
       <x:c r="A3" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -606,7 +516,7 @@
         <x:v>14</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:12">
+    <x:row r="4" spans="1:10">
       <x:c r="A4" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
@@ -626,7 +536,7 @@
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:12">
+    <x:row r="5" spans="1:10">
       <x:c r="A5" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
@@ -646,7 +556,7 @@
         <x:v>20</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:12">
+    <x:row r="6" spans="1:10">
       <x:c r="A6" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
@@ -666,7 +576,7 @@
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:12">
+    <x:row r="7" spans="1:10">
       <x:c r="A7" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
@@ -686,12 +596,12 @@
         <x:v>26</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:12">
+    <x:row r="8" spans="1:10">
       <x:c r="A8" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
         <x:v>8</x:v>
@@ -703,187 +613,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:12">
-      <x:c r="A9" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="C9" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E9" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F9" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:12">
-      <x:c r="A10" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="C10" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E10" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F10" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:12">
-      <x:c r="A11" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="C11" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D11" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E11" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F11" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:12">
-      <x:c r="A12" s="0" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="C12" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E12" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="F12" s="0" t="s">
-        <x:v>42</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:12">
-      <x:c r="A13" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="B13" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="C13" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D13" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E13" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="F13" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:12">
-      <x:c r="A14" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="B14" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="C14" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D14" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E14" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="F14" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:12">
-      <x:c r="A15" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="B15" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="C15" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D15" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E15" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="F15" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:12">
-      <x:c r="A16" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D16" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E16" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="F16" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:12">
-      <x:c r="A17" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="B17" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D17" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E17" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="F17" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>